<commit_message>
BIS-769: Fixed propertytype error handling; improvements to migration script
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t xml:space="preserve">SAMPLE_TYPE</t>
   </si>
@@ -240,7 +240,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,10 +270,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -297,10 +293,10 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4:N4"/>
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="26.5"/>
   </cols>
@@ -430,9 +426,8 @@
       <c r="K5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="8" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L5" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,9 +460,8 @@
       <c r="K6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="8" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L6" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,9 +492,8 @@
       <c r="K7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="8" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="L7" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>